<commit_message>
initial stuff on clinical trials.
</commit_message>
<xml_diff>
--- a/tabular/contributed/clinicalTrials.xlsx
+++ b/tabular/contributed/clinicalTrials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16340" yWindow="4840" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="25660" yWindow="6620" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>displayName</t>
-  </si>
-  <si>
     <t>regimen</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>GS-US-367-1871</t>
+  </si>
+  <si>
+    <t>display_name</t>
   </si>
 </sst>
 </file>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,285 +487,285 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed addition of elbasvir resistance data.
Tweak to report generation to ensure summary is sorted by category.

Code to load in resistance findings made slightly more robust.
</commit_message>
<xml_diff>
--- a/tabular/contributed/clinicalTrials.xlsx
+++ b/tabular/contributed/clinicalTrials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34420" yWindow="2860" windowWidth="15040" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="21460" yWindow="13460" windowWidth="26940" windowHeight="13060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -354,16 +354,128 @@
   </si>
   <si>
     <t>nct_id</t>
+  </si>
+  <si>
+    <t>C-WORTHY</t>
+  </si>
+  <si>
+    <t>NCT01717326</t>
+  </si>
+  <si>
+    <t>NCT02105454</t>
+  </si>
+  <si>
+    <t>C-SALVAGE</t>
+  </si>
+  <si>
+    <t>C-EDGE CO-INFECTION</t>
+  </si>
+  <si>
+    <t>NCT02105662</t>
+  </si>
+  <si>
+    <t>NCT02105701</t>
+  </si>
+  <si>
+    <t>C-EDGE TE</t>
+  </si>
+  <si>
+    <t>NCT02203149</t>
+  </si>
+  <si>
+    <t>C-WORTHY Part D</t>
+  </si>
+  <si>
+    <t>C-SURFER</t>
+  </si>
+  <si>
+    <t>NCT02092350</t>
+  </si>
+  <si>
+    <t>NCT02601573</t>
+  </si>
+  <si>
+    <t>C-ISLE</t>
+  </si>
+  <si>
+    <t>Swiss HCVree</t>
+  </si>
+  <si>
+    <t>NCT02785666</t>
+  </si>
+  <si>
+    <t>C-EDGE CO-STAR</t>
+  </si>
+  <si>
+    <t>NCT02105688</t>
+  </si>
+  <si>
+    <t>C-WORTHy Part D</t>
+  </si>
+  <si>
+    <t>C-WORTHy</t>
+  </si>
+  <si>
+    <t>C-EDGE TN</t>
+  </si>
+  <si>
+    <t>NCT02105467</t>
+  </si>
+  <si>
+    <t>C‐SCAPE </t>
+  </si>
+  <si>
+    <t>NCT01932762</t>
+  </si>
+  <si>
+    <t>NCT02252016</t>
+  </si>
+  <si>
+    <t>C‐EDGE Head‐2‐head</t>
+  </si>
+  <si>
+    <t>NCT02358044</t>
+  </si>
+  <si>
+    <t>NCT02251990</t>
+  </si>
+  <si>
+    <t>C-CORAL</t>
+  </si>
+  <si>
+    <t>C‐EDGE IBLD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -383,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -391,11 +503,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,8 +550,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,15 +840,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A29" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
@@ -1291,6 +1448,171 @@
         <v>107</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more work on DCV / LDV / EBR / VEL
</commit_message>
<xml_diff>
--- a/tabular/contributed/clinicalTrials.xlsx
+++ b/tabular/contributed/clinicalTrials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21460" yWindow="13460" windowWidth="26940" windowHeight="13060" tabRatio="500"/>
+    <workbookView xWindow="-21400" yWindow="2040" windowWidth="20480" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="161">
   <si>
     <t>id</t>
   </si>
@@ -444,6 +444,72 @@
   </si>
   <si>
     <t>C‐EDGE IBLD</t>
+  </si>
+  <si>
+    <t>HEPATHER</t>
+  </si>
+  <si>
+    <t>NCT01953458</t>
+  </si>
+  <si>
+    <t>NCT02600351</t>
+  </si>
+  <si>
+    <t>RESCUE</t>
+  </si>
+  <si>
+    <t>NCT01012895</t>
+  </si>
+  <si>
+    <t>NCT01628692</t>
+  </si>
+  <si>
+    <t>NCT02319031</t>
+  </si>
+  <si>
+    <t>ALLY-3</t>
+  </si>
+  <si>
+    <t>NCT01581203</t>
+  </si>
+  <si>
+    <t>Hallmark DUAL</t>
+  </si>
+  <si>
+    <t>NCT01995266</t>
+  </si>
+  <si>
+    <t>NCT02496078</t>
+  </si>
+  <si>
+    <t>DUAL</t>
+  </si>
+  <si>
+    <t>NCT01497834</t>
+  </si>
+  <si>
+    <t>NCT01718145</t>
+  </si>
+  <si>
+    <t>NCT01051414</t>
+  </si>
+  <si>
+    <t>UMIN000015627</t>
+  </si>
+  <si>
+    <t>NCT01257204</t>
+  </si>
+  <si>
+    <t>NCT01359644</t>
+  </si>
+  <si>
+    <t>NCT02032875</t>
+  </si>
+  <si>
+    <t>NCT01616524</t>
+  </si>
+  <si>
+    <t>NCT01492504</t>
   </si>
 </sst>
 </file>
@@ -840,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1613,6 +1679,201 @@
         <v>136</v>
       </c>
     </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>156</v>
+      </c>
+      <c r="B82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>158</v>
+      </c>
+      <c r="B84" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some new RASs from BOSON study article.
</commit_message>
<xml_diff>
--- a/tabular/contributed/clinicalTrials.xlsx
+++ b/tabular/contributed/clinicalTrials.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22000" yWindow="6040" windowWidth="19100" windowHeight="20760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49840" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="190">
   <si>
     <t>id</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>NCT02265237</t>
+  </si>
+  <si>
+    <t>BOSON</t>
+  </si>
+  <si>
+    <t>NCT01962441</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:XFD104"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2139,6 +2145,17 @@
         <v>177</v>
       </c>
     </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>